<commit_message>
Aligning create_timeseries.py and build_input_excel.py definitions and interfaces, allowing flexible Backbone dimensions to timeseries_specs, adding scenario alternatives
</commit_message>
<xml_diff>
--- a/src_files/demands_DH_own_projection.xlsx
+++ b/src_files/demands_DH_own_projection.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BB\bb-master\north_european_model\src_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD27828B-3730-4F20-AEF5-438994C7157E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FED8F2BE-58D9-456E-8D39-6939ED2BAFCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="854" xr2:uid="{3FAE13E1-8810-491E-8373-B01BC9956BE7}"/>
+    <workbookView xWindow="-28920" yWindow="-105" windowWidth="29040" windowHeight="17520" tabRatio="854" activeTab="6" xr2:uid="{3FAE13E1-8810-491E-8373-B01BC9956BE7}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="14" r:id="rId1"/>
@@ -128,7 +128,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1387" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1387" uniqueCount="353">
   <si>
     <t>Total (GWh)</t>
   </si>
@@ -1270,6 +1270,9 @@
   <si>
     <t>Duplicate entries in any of the sheets</t>
   </si>
+  <si>
+    <t>dheat</t>
+  </si>
 </sst>
 </file>
 
@@ -1303,28 +1306,33 @@
     <font>
       <sz val="9"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color indexed="9"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="9"/>
       <color indexed="12"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -25190,8 +25198,8 @@
   </sheetPr>
   <dimension ref="B4:D45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -40670,7 +40678,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J27" sqref="J27"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -40715,7 +40723,7 @@
       </c>
       <c r="B2" t="str">
         <f>IF(Finland!C5="","",Finland!C5)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C2" t="str">
         <f>IF(Finland!D5="","",Finland!D5)</f>
@@ -40745,7 +40753,7 @@
       </c>
       <c r="B3" t="str">
         <f>IF(Finland!C6="","",Finland!C6)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C3" t="str">
         <f>IF(Finland!D6="","",Finland!D6)</f>
@@ -40775,7 +40783,7 @@
       </c>
       <c r="B4" t="str">
         <f>IF(Finland!C7="","",Finland!C7)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C4" t="str">
         <f>IF(Finland!D7="","",Finland!D7)</f>
@@ -40805,7 +40813,7 @@
       </c>
       <c r="B5" t="str">
         <f>IF(Finland!C8="","",Finland!C8)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C5" t="str">
         <f>IF(Finland!D8="","",Finland!D8)</f>
@@ -40835,7 +40843,7 @@
       </c>
       <c r="B6" t="str">
         <f>IF(Finland!C9="","",Finland!C9)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C6" t="str">
         <f>IF(Finland!D9="","",Finland!D9)</f>
@@ -40865,7 +40873,7 @@
       </c>
       <c r="B7" t="str">
         <f>IF(Finland!C10="","",Finland!C10)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C7" t="str">
         <f>IF(Finland!D10="","",Finland!D10)</f>
@@ -40895,7 +40903,7 @@
       </c>
       <c r="B8" t="str">
         <f>IF(Finland!C11="","",Finland!C11)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C8" t="str">
         <f>IF(Finland!D11="","",Finland!D11)</f>
@@ -40925,7 +40933,7 @@
       </c>
       <c r="B9" t="str">
         <f>IF(Finland!C12="","",Finland!C12)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C9" t="str">
         <f>IF(Finland!D12="","",Finland!D12)</f>
@@ -40955,7 +40963,7 @@
       </c>
       <c r="B10" t="str">
         <f>IF(Finland!C13="","",Finland!C13)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C10" t="str">
         <f>IF(Finland!D13="","",Finland!D13)</f>
@@ -40985,7 +40993,7 @@
       </c>
       <c r="B11" t="str">
         <f>IF(Finland!C14="","",Finland!C14)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C11" t="str">
         <f>IF(Finland!D14="","",Finland!D14)</f>
@@ -41015,7 +41023,7 @@
       </c>
       <c r="B12" t="str">
         <f>IF(Finland!C15="","",Finland!C15)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C12" t="str">
         <f>IF(Finland!D15="","",Finland!D15)</f>
@@ -41045,7 +41053,7 @@
       </c>
       <c r="B13" t="str">
         <f>IF(Finland!C16="","",Finland!C16)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C13" t="str">
         <f>IF(Finland!D16="","",Finland!D16)</f>
@@ -41075,7 +41083,7 @@
       </c>
       <c r="B14" t="str">
         <f>IF(Finland!C17="","",Finland!C17)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C14" t="str">
         <f>IF(Finland!D17="","",Finland!D17)</f>
@@ -41105,7 +41113,7 @@
       </c>
       <c r="B15" t="str">
         <f>IF(Finland!C18="","",Finland!C18)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C15" t="str">
         <f>IF(Finland!D18="","",Finland!D18)</f>
@@ -41135,7 +41143,7 @@
       </c>
       <c r="B16" t="str">
         <f>IF(Finland!C19="","",Finland!C19)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C16" t="str">
         <f>IF(Finland!D19="","",Finland!D19)</f>
@@ -41165,7 +41173,7 @@
       </c>
       <c r="B17" t="str">
         <f>IF(Finland!C20="","",Finland!C20)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C17" t="str">
         <f>IF(Finland!D20="","",Finland!D20)</f>
@@ -41195,7 +41203,7 @@
       </c>
       <c r="B18" t="str">
         <f>IF(Finland!C21="","",Finland!C21)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C18" t="str">
         <f>IF(Finland!D21="","",Finland!D21)</f>
@@ -41225,7 +41233,7 @@
       </c>
       <c r="B19" t="str">
         <f>IF(Finland!C22="","",Finland!C22)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C19" t="str">
         <f>IF(Finland!D22="","",Finland!D22)</f>
@@ -41255,7 +41263,7 @@
       </c>
       <c r="B20" t="str">
         <f>IF(Finland!C23="","",Finland!C23)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C20" t="str">
         <f>IF(Finland!D23="","",Finland!D23)</f>
@@ -41285,7 +41293,7 @@
       </c>
       <c r="B21" t="str">
         <f>IF(Finland!C24="","",Finland!C24)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C21" t="str">
         <f>IF(Finland!D24="","",Finland!D24)</f>
@@ -41315,7 +41323,7 @@
       </c>
       <c r="B22" t="str">
         <f>IF(Finland!C25="","",Finland!C25)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C22" t="str">
         <f>IF(Finland!D25="","",Finland!D25)</f>
@@ -41345,7 +41353,7 @@
       </c>
       <c r="B23" t="str">
         <f>IF(Finland!C26="","",Finland!C26)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C23" t="str">
         <f>IF(Finland!D26="","",Finland!D26)</f>
@@ -41375,7 +41383,7 @@
       </c>
       <c r="B24" t="str">
         <f>IF(Finland!C27="","",Finland!C27)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C24" t="str">
         <f>IF(Finland!D27="","",Finland!D27)</f>
@@ -41405,7 +41413,7 @@
       </c>
       <c r="B25" t="str">
         <f>IF(Finland!C28="","",Finland!C28)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C25" t="str">
         <f>IF(Finland!D28="","",Finland!D28)</f>
@@ -41435,7 +41443,7 @@
       </c>
       <c r="B26" t="str">
         <f>IF(Finland!C29="","",Finland!C29)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C26" t="str">
         <f>IF(Finland!D29="","",Finland!D29)</f>
@@ -41465,7 +41473,7 @@
       </c>
       <c r="B27" t="str">
         <f>IF(Finland!C30="","",Finland!C30)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C27" t="str">
         <f>IF(Finland!D30="","",Finland!D30)</f>
@@ -41495,7 +41503,7 @@
       </c>
       <c r="B28" t="str">
         <f>IF(Finland!C31="","",Finland!C31)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C28" t="str">
         <f>IF(Finland!D31="","",Finland!D31)</f>
@@ -41525,7 +41533,7 @@
       </c>
       <c r="B29" t="str">
         <f>IF(Finland!C32="","",Finland!C32)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C29" t="str">
         <f>IF(Finland!D32="","",Finland!D32)</f>
@@ -41555,7 +41563,7 @@
       </c>
       <c r="B30" t="str">
         <f>IF(Finland!C33="","",Finland!C33)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C30" t="str">
         <f>IF(Finland!D33="","",Finland!D33)</f>
@@ -41585,7 +41593,7 @@
       </c>
       <c r="B31" t="str">
         <f>IF(Finland!C34="","",Finland!C34)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C31" t="str">
         <f>IF(Finland!D34="","",Finland!D34)</f>
@@ -41615,7 +41623,7 @@
       </c>
       <c r="B32" t="str">
         <f>IF(Finland!C35="","",Finland!C35)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C32" t="str">
         <f>IF(Finland!D35="","",Finland!D35)</f>
@@ -41645,7 +41653,7 @@
       </c>
       <c r="B33" t="str">
         <f>IF(Finland!C36="","",Finland!C36)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C33" t="str">
         <f>IF(Finland!D36="","",Finland!D36)</f>
@@ -41675,7 +41683,7 @@
       </c>
       <c r="B34" t="str">
         <f>IF(Norway!C5="","", Norway!C5)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C34" t="str">
         <f>IF(Norway!D5="","", Norway!D5)</f>
@@ -41705,7 +41713,7 @@
       </c>
       <c r="B35" t="str">
         <f>IF(Norway!C6="","", Norway!C6)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C35" t="str">
         <f>IF(Norway!D6="","", Norway!D6)</f>
@@ -41735,7 +41743,7 @@
       </c>
       <c r="B36" t="str">
         <f>IF(Norway!C7="","", Norway!C7)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C36" t="str">
         <f>IF(Norway!D7="","", Norway!D7)</f>
@@ -41765,7 +41773,7 @@
       </c>
       <c r="B37" t="str">
         <f>IF(Norway!C8="","", Norway!C8)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C37" t="str">
         <f>IF(Norway!D8="","", Norway!D8)</f>
@@ -41795,7 +41803,7 @@
       </c>
       <c r="B38" t="str">
         <f>IF(Norway!C9="","", Norway!C9)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C38" t="str">
         <f>IF(Norway!D9="","", Norway!D9)</f>
@@ -41825,7 +41833,7 @@
       </c>
       <c r="B39" t="str">
         <f>IF(Norway!C10="","", Norway!C10)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C39" t="str">
         <f>IF(Norway!D10="","", Norway!D10)</f>
@@ -41855,7 +41863,7 @@
       </c>
       <c r="B40" t="str">
         <f>IF(Norway!C11="","", Norway!C11)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C40" t="str">
         <f>IF(Norway!D11="","", Norway!D11)</f>
@@ -41885,7 +41893,7 @@
       </c>
       <c r="B41" t="str">
         <f>IF(Norway!C12="","", Norway!C12)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C41" t="str">
         <f>IF(Norway!D12="","", Norway!D12)</f>
@@ -41915,7 +41923,7 @@
       </c>
       <c r="B42" t="str">
         <f>IF(Norway!C13="","", Norway!C13)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C42" t="str">
         <f>IF(Norway!D13="","", Norway!D13)</f>
@@ -41945,7 +41953,7 @@
       </c>
       <c r="B43" t="str">
         <f>IF(Norway!C14="","", Norway!C14)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C43" t="str">
         <f>IF(Norway!D14="","", Norway!D14)</f>
@@ -41975,7 +41983,7 @@
       </c>
       <c r="B44" t="str">
         <f>IF(Norway!C15="","", Norway!C15)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C44" t="str">
         <f>IF(Norway!D15="","", Norway!D15)</f>
@@ -42005,7 +42013,7 @@
       </c>
       <c r="B45" t="str">
         <f>IF(Norway!C16="","", Norway!C16)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C45" t="str">
         <f>IF(Norway!D16="","", Norway!D16)</f>
@@ -42035,7 +42043,7 @@
       </c>
       <c r="B46" t="str">
         <f>IF(Sweden!C5="","",Sweden!C5)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C46" t="str">
         <f>IF(Sweden!D5="","",Sweden!D5)</f>
@@ -42065,7 +42073,7 @@
       </c>
       <c r="B47" t="str">
         <f>IF(Sweden!C6="","",Sweden!C6)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C47" t="str">
         <f>IF(Sweden!D6="","",Sweden!D6)</f>
@@ -42095,7 +42103,7 @@
       </c>
       <c r="B48" t="str">
         <f>IF(Sweden!C7="","",Sweden!C7)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C48" t="str">
         <f>IF(Sweden!D7="","",Sweden!D7)</f>
@@ -42125,7 +42133,7 @@
       </c>
       <c r="B49" t="str">
         <f>IF(Sweden!C8="","",Sweden!C8)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C49" t="str">
         <f>IF(Sweden!D8="","",Sweden!D8)</f>
@@ -42155,7 +42163,7 @@
       </c>
       <c r="B50" t="str">
         <f>IF(Sweden!C9="","",Sweden!C9)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C50" t="str">
         <f>IF(Sweden!D9="","",Sweden!D9)</f>
@@ -42185,7 +42193,7 @@
       </c>
       <c r="B51" t="str">
         <f>IF(Sweden!C10="","",Sweden!C10)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C51" t="str">
         <f>IF(Sweden!D10="","",Sweden!D10)</f>
@@ -42215,7 +42223,7 @@
       </c>
       <c r="B52" t="str">
         <f>IF(Sweden!C11="","",Sweden!C11)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C52" t="str">
         <f>IF(Sweden!D11="","",Sweden!D11)</f>
@@ -42245,7 +42253,7 @@
       </c>
       <c r="B53" t="str">
         <f>IF(Sweden!C12="","",Sweden!C12)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C53" t="str">
         <f>IF(Sweden!D12="","",Sweden!D12)</f>
@@ -42275,7 +42283,7 @@
       </c>
       <c r="B54" t="str">
         <f>IF(Sweden!C13="","",Sweden!C13)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C54" t="str">
         <f>IF(Sweden!D13="","",Sweden!D13)</f>
@@ -42305,7 +42313,7 @@
       </c>
       <c r="B55" t="str">
         <f>IF(Sweden!C14="","",Sweden!C14)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C55" t="str">
         <f>IF(Sweden!D14="","",Sweden!D14)</f>
@@ -42335,7 +42343,7 @@
       </c>
       <c r="B56" t="str">
         <f>IF(Sweden!C15="","",Sweden!C15)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C56" t="str">
         <f>IF(Sweden!D15="","",Sweden!D15)</f>
@@ -42365,7 +42373,7 @@
       </c>
       <c r="B57" t="str">
         <f>IF(Sweden!C16="","",Sweden!C16)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C57" t="str">
         <f>IF(Sweden!D16="","",Sweden!D16)</f>
@@ -42395,7 +42403,7 @@
       </c>
       <c r="B58" t="str">
         <f>IF(Sweden!C17="","",Sweden!C17)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C58" t="str">
         <f>IF(Sweden!D17="","",Sweden!D17)</f>
@@ -42425,7 +42433,7 @@
       </c>
       <c r="B59" t="str">
         <f>IF(Sweden!C18="","",Sweden!C18)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C59" t="str">
         <f>IF(Sweden!D18="","",Sweden!D18)</f>
@@ -42455,7 +42463,7 @@
       </c>
       <c r="B60" t="str">
         <f>IF(Sweden!C19="","",Sweden!C19)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C60" t="str">
         <f>IF(Sweden!D19="","",Sweden!D19)</f>
@@ -42485,7 +42493,7 @@
       </c>
       <c r="B61" t="str">
         <f>IF(Sweden!C20="","",Sweden!C20)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C61" t="str">
         <f>IF(Sweden!D20="","",Sweden!D20)</f>
@@ -42515,7 +42523,7 @@
       </c>
       <c r="B62" t="str">
         <f>IF(Denmark!C5="","",Denmark!C5)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C62" t="str">
         <f>IF(Denmark!D5="","",Denmark!D5)</f>
@@ -42545,7 +42553,7 @@
       </c>
       <c r="B63" t="str">
         <f>IF(Denmark!C6="","",Denmark!C6)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C63" t="str">
         <f>IF(Denmark!D6="","",Denmark!D6)</f>
@@ -42575,7 +42583,7 @@
       </c>
       <c r="B64" t="str">
         <f>IF(Denmark!C7="","",Denmark!C7)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C64" t="str">
         <f>IF(Denmark!D7="","",Denmark!D7)</f>
@@ -42605,7 +42613,7 @@
       </c>
       <c r="B65" t="str">
         <f>IF(Denmark!C8="","",Denmark!C8)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C65" t="str">
         <f>IF(Denmark!D8="","",Denmark!D8)</f>
@@ -42635,7 +42643,7 @@
       </c>
       <c r="B66" t="str">
         <f>IF(Denmark!C9="","",Denmark!C9)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C66" t="str">
         <f>IF(Denmark!D9="","",Denmark!D9)</f>
@@ -42665,7 +42673,7 @@
       </c>
       <c r="B67" t="str">
         <f>IF(Denmark!C10="","",Denmark!C10)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C67" t="str">
         <f>IF(Denmark!D10="","",Denmark!D10)</f>
@@ -42695,7 +42703,7 @@
       </c>
       <c r="B68" t="str">
         <f>IF(Denmark!C11="","",Denmark!C11)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C68" t="str">
         <f>IF(Denmark!D11="","",Denmark!D11)</f>
@@ -42725,7 +42733,7 @@
       </c>
       <c r="B69" t="str">
         <f>IF(Denmark!C12="","",Denmark!C12)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C69" t="str">
         <f>IF(Denmark!D12="","",Denmark!D12)</f>
@@ -42755,7 +42763,7 @@
       </c>
       <c r="B70" t="str">
         <f>IF(others!C5="","",others!C5)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C70" t="str">
         <f>IF(others!D5="","",others!D5)</f>
@@ -42785,7 +42793,7 @@
       </c>
       <c r="B71" t="str">
         <f>IF(others!C6="","",others!C6)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C71" t="str">
         <f>IF(others!D6="","",others!D6)</f>
@@ -42815,7 +42823,7 @@
       </c>
       <c r="B72" t="str">
         <f>IF(others!C7="","",others!C7)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C72" t="str">
         <f>IF(others!D7="","",others!D7)</f>
@@ -42845,7 +42853,7 @@
       </c>
       <c r="B73" t="str">
         <f>IF(others!C8="","",others!C8)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C73" t="str">
         <f>IF(others!D8="","",others!D8)</f>
@@ -42875,7 +42883,7 @@
       </c>
       <c r="B74" t="str">
         <f>IF(others!C9="","",others!C9)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C74" t="str">
         <f>IF(others!D9="","",others!D9)</f>
@@ -42905,7 +42913,7 @@
       </c>
       <c r="B75" t="str">
         <f>IF(others!C10="","",others!C10)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C75" t="str">
         <f>IF(others!D10="","",others!D10)</f>
@@ -42935,7 +42943,7 @@
       </c>
       <c r="B76" t="str">
         <f>IF(others!C11="","",others!C11)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C76" t="str">
         <f>IF(others!D11="","",others!D11)</f>
@@ -42965,7 +42973,7 @@
       </c>
       <c r="B77" t="str">
         <f>IF(others!C12="","",others!C12)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C77" t="str">
         <f>IF(others!D12="","",others!D12)</f>
@@ -42995,7 +43003,7 @@
       </c>
       <c r="B78" t="str">
         <f>IF(others!C13="","",others!C13)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C78" t="str">
         <f>IF(others!D13="","",others!D13)</f>
@@ -43025,7 +43033,7 @@
       </c>
       <c r="B79" t="str">
         <f>IF(others!C14="","",others!C14)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C79" t="str">
         <f>IF(others!D14="","",others!D14)</f>
@@ -43055,7 +43063,7 @@
       </c>
       <c r="B80" t="str">
         <f>IF(others!C15="","",others!C15)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C80" t="str">
         <f>IF(others!D15="","",others!D15)</f>
@@ -43085,7 +43093,7 @@
       </c>
       <c r="B81" t="str">
         <f>IF(others!C16="","",others!C16)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C81" t="str">
         <f>IF(others!D16="","",others!D16)</f>
@@ -43115,7 +43123,7 @@
       </c>
       <c r="B82" t="str">
         <f>IF(others!C17="","",others!C17)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C82" t="str">
         <f>IF(others!D17="","",others!D17)</f>
@@ -43145,7 +43153,7 @@
       </c>
       <c r="B83" t="str">
         <f>IF(others!C18="","",others!C18)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C83" t="str">
         <f>IF(others!D18="","",others!D18)</f>
@@ -43175,7 +43183,7 @@
       </c>
       <c r="B84" t="str">
         <f>IF(others!C19="","",others!C19)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C84" t="str">
         <f>IF(others!D19="","",others!D19)</f>
@@ -43205,7 +43213,7 @@
       </c>
       <c r="B85" t="str">
         <f>IF(others!C20="","",others!C20)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C85" t="str">
         <f>IF(others!D20="","",others!D20)</f>
@@ -43235,7 +43243,7 @@
       </c>
       <c r="B86" t="str">
         <f>IF(others!C21="","",others!C21)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C86" t="str">
         <f>IF(others!D21="","",others!D21)</f>
@@ -43265,7 +43273,7 @@
       </c>
       <c r="B87" t="str">
         <f>IF(others!C22="","",others!C22)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C87" t="str">
         <f>IF(others!D22="","",others!D22)</f>
@@ -43295,7 +43303,7 @@
       </c>
       <c r="B88" t="str">
         <f>IF(others!C23="","",others!C23)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C88" t="str">
         <f>IF(others!D23="","",others!D23)</f>
@@ -43325,7 +43333,7 @@
       </c>
       <c r="B89" t="str">
         <f>IF(others!C24="","",others!C24)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C89" t="str">
         <f>IF(others!D24="","",others!D24)</f>
@@ -43355,7 +43363,7 @@
       </c>
       <c r="B90" t="str">
         <f>IF(others!C25="","",others!C25)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C90" t="str">
         <f>IF(others!D25="","",others!D25)</f>
@@ -43385,7 +43393,7 @@
       </c>
       <c r="B91" t="str">
         <f>IF(others!C26="","",others!C26)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C91" t="str">
         <f>IF(others!D26="","",others!D26)</f>
@@ -43415,7 +43423,7 @@
       </c>
       <c r="B92" t="str">
         <f>IF(others!C27="","",others!C27)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C92" t="str">
         <f>IF(others!D27="","",others!D27)</f>
@@ -43445,7 +43453,7 @@
       </c>
       <c r="B93" t="str">
         <f>IF(others!C28="","",others!C28)</f>
-        <v>heat</v>
+        <v>dheat</v>
       </c>
       <c r="C93" t="str">
         <f>IF(others!D28="","",others!D28)</f>
@@ -43486,7 +43494,7 @@
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection activeCell="L27" sqref="L27"/>
-      <selection pane="topRight" activeCell="L27" sqref="L27"/>
+      <selection pane="topRight" activeCell="P18" sqref="P18:P19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -43555,7 +43563,7 @@
         <v>177</v>
       </c>
       <c r="C5" s="70" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D5" s="70" t="s">
         <v>297</v>
@@ -43592,7 +43600,7 @@
         <v>177</v>
       </c>
       <c r="C6" s="75" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D6" s="75" t="s">
         <v>298</v>
@@ -43636,7 +43644,7 @@
         <v>177</v>
       </c>
       <c r="C7" s="70" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D7" s="70" t="s">
         <v>299</v>
@@ -43680,7 +43688,7 @@
         <v>177</v>
       </c>
       <c r="C8" s="75" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D8" s="75" t="s">
         <v>300</v>
@@ -43724,7 +43732,7 @@
         <v>177</v>
       </c>
       <c r="C9" s="70" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D9" s="70" t="s">
         <v>301</v>
@@ -43768,7 +43776,7 @@
         <v>177</v>
       </c>
       <c r="C10" s="75" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D10" s="75" t="s">
         <v>302</v>
@@ -43812,7 +43820,7 @@
         <v>177</v>
       </c>
       <c r="C11" s="70" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D11" s="70" t="s">
         <v>303</v>
@@ -43856,7 +43864,7 @@
         <v>177</v>
       </c>
       <c r="C12" s="75" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D12" s="75" t="s">
         <v>304</v>
@@ -43900,7 +43908,7 @@
         <v>177</v>
       </c>
       <c r="C13" s="70" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D13" s="70" t="s">
         <v>297</v>
@@ -43945,7 +43953,7 @@
         <v>177</v>
       </c>
       <c r="C14" s="75" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D14" s="75" t="s">
         <v>298</v>
@@ -43971,7 +43979,7 @@
         <v>177</v>
       </c>
       <c r="C15" s="70" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D15" s="70" t="s">
         <v>299</v>
@@ -43997,7 +44005,7 @@
         <v>177</v>
       </c>
       <c r="C16" s="75" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D16" s="75" t="s">
         <v>300</v>
@@ -44023,7 +44031,7 @@
         <v>177</v>
       </c>
       <c r="C17" s="70" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D17" s="70" t="s">
         <v>301</v>
@@ -44049,7 +44057,7 @@
         <v>177</v>
       </c>
       <c r="C18" s="75" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D18" s="75" t="s">
         <v>302</v>
@@ -44075,7 +44083,7 @@
         <v>177</v>
       </c>
       <c r="C19" s="70" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D19" s="70" t="s">
         <v>303</v>
@@ -44101,7 +44109,7 @@
         <v>177</v>
       </c>
       <c r="C20" s="75" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D20" s="75" t="s">
         <v>304</v>
@@ -44127,7 +44135,7 @@
         <v>177</v>
       </c>
       <c r="C21" s="70" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D21" s="70" t="s">
         <v>297</v>
@@ -44153,7 +44161,7 @@
         <v>177</v>
       </c>
       <c r="C22" s="75" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D22" s="75" t="s">
         <v>298</v>
@@ -44179,7 +44187,7 @@
         <v>177</v>
       </c>
       <c r="C23" s="70" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D23" s="70" t="s">
         <v>299</v>
@@ -44205,7 +44213,7 @@
         <v>177</v>
       </c>
       <c r="C24" s="75" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D24" s="75" t="s">
         <v>300</v>
@@ -44231,7 +44239,7 @@
         <v>177</v>
       </c>
       <c r="C25" s="70" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D25" s="70" t="s">
         <v>301</v>
@@ -44257,7 +44265,7 @@
         <v>177</v>
       </c>
       <c r="C26" s="75" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D26" s="75" t="s">
         <v>302</v>
@@ -44283,7 +44291,7 @@
         <v>177</v>
       </c>
       <c r="C27" s="70" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D27" s="70" t="s">
         <v>303</v>
@@ -44309,7 +44317,7 @@
         <v>177</v>
       </c>
       <c r="C28" s="75" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D28" s="75" t="s">
         <v>304</v>
@@ -44335,7 +44343,7 @@
         <v>177</v>
       </c>
       <c r="C29" s="70" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D29" s="70" t="s">
         <v>297</v>
@@ -44361,7 +44369,7 @@
         <v>177</v>
       </c>
       <c r="C30" s="75" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D30" s="75" t="s">
         <v>298</v>
@@ -44387,7 +44395,7 @@
         <v>177</v>
       </c>
       <c r="C31" s="70" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D31" s="70" t="s">
         <v>299</v>
@@ -44413,7 +44421,7 @@
         <v>177</v>
       </c>
       <c r="C32" s="75" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D32" s="75" t="s">
         <v>300</v>
@@ -44439,7 +44447,7 @@
         <v>177</v>
       </c>
       <c r="C33" s="70" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D33" s="70" t="s">
         <v>301</v>
@@ -44465,7 +44473,7 @@
         <v>177</v>
       </c>
       <c r="C34" s="75" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D34" s="75" t="s">
         <v>302</v>
@@ -44491,7 +44499,7 @@
         <v>177</v>
       </c>
       <c r="C35" s="70" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D35" s="70" t="s">
         <v>303</v>
@@ -44517,7 +44525,7 @@
         <v>177</v>
       </c>
       <c r="C36" s="75" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D36" s="75" t="s">
         <v>304</v>
@@ -51639,7 +51647,7 @@
   <dimension ref="A1:AQ86"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L27" sqref="L27"/>
+      <selection activeCell="C5" sqref="C5:C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -51684,7 +51692,7 @@
         <v>167</v>
       </c>
       <c r="C5" s="70" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D5" s="70"/>
       <c r="E5" s="70" t="s">
@@ -51713,7 +51721,7 @@
         <v>168</v>
       </c>
       <c r="C6" s="75" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D6" s="75"/>
       <c r="E6" s="75" t="s">
@@ -51743,7 +51751,7 @@
         <v>169</v>
       </c>
       <c r="C7" s="70" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D7" s="70"/>
       <c r="E7" s="70" t="s">
@@ -51773,7 +51781,7 @@
         <v>167</v>
       </c>
       <c r="C8" s="75" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D8" s="75"/>
       <c r="E8" s="75" t="s">
@@ -51803,7 +51811,7 @@
         <v>168</v>
       </c>
       <c r="C9" s="70" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D9" s="70"/>
       <c r="E9" s="70" t="s">
@@ -51826,7 +51834,7 @@
         <v>169</v>
       </c>
       <c r="C10" s="75" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D10" s="75"/>
       <c r="E10" s="75" t="s">
@@ -51861,7 +51869,7 @@
         <v>167</v>
       </c>
       <c r="C11" s="70" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D11" s="70"/>
       <c r="E11" s="70" t="s">
@@ -51903,7 +51911,7 @@
         <v>168</v>
       </c>
       <c r="C12" s="75" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D12" s="75"/>
       <c r="E12" s="75" t="s">
@@ -51926,7 +51934,7 @@
         <v>169</v>
       </c>
       <c r="C13" s="70" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D13" s="70"/>
       <c r="E13" s="70" t="s">
@@ -51949,7 +51957,7 @@
         <v>167</v>
       </c>
       <c r="C14" s="75" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D14" s="75"/>
       <c r="E14" s="75" t="s">
@@ -51972,7 +51980,7 @@
         <v>168</v>
       </c>
       <c r="C15" s="70" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D15" s="70"/>
       <c r="E15" s="70" t="s">
@@ -51998,7 +52006,7 @@
         <v>169</v>
       </c>
       <c r="C16" s="75" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D16" s="75"/>
       <c r="E16" s="75" t="s">
@@ -55013,7 +55021,7 @@
   <dimension ref="B1:R110"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L27" sqref="L27"/>
+      <selection activeCell="C5" sqref="C5:C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -55058,7 +55066,7 @@
         <v>189</v>
       </c>
       <c r="C5" s="70" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D5" s="70"/>
       <c r="E5" s="70" t="s">
@@ -55083,7 +55091,7 @@
         <v>194</v>
       </c>
       <c r="C6" s="75" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D6" s="75"/>
       <c r="E6" s="75" t="s">
@@ -55106,7 +55114,7 @@
         <v>207</v>
       </c>
       <c r="C7" s="70" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D7" s="70"/>
       <c r="E7" s="70" t="s">
@@ -55135,7 +55143,7 @@
         <v>212</v>
       </c>
       <c r="C8" s="75" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D8" s="75"/>
       <c r="E8" s="75" t="s">
@@ -55169,7 +55177,7 @@
         <v>189</v>
       </c>
       <c r="C9" s="70" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D9" s="70"/>
       <c r="E9" s="70" t="s">
@@ -55204,7 +55212,7 @@
         <v>194</v>
       </c>
       <c r="C10" s="75" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D10" s="75"/>
       <c r="E10" s="75" t="s">
@@ -55241,7 +55249,7 @@
         <v>207</v>
       </c>
       <c r="C11" s="70" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D11" s="70"/>
       <c r="E11" s="70" t="s">
@@ -55276,7 +55284,7 @@
         <v>212</v>
       </c>
       <c r="C12" s="75" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D12" s="75"/>
       <c r="E12" s="75" t="s">
@@ -55300,7 +55308,7 @@
         <v>189</v>
       </c>
       <c r="C13" s="70" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D13" s="70"/>
       <c r="E13" s="70" t="s">
@@ -55324,7 +55332,7 @@
         <v>194</v>
       </c>
       <c r="C14" s="75" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D14" s="75"/>
       <c r="E14" s="75" t="s">
@@ -55360,7 +55368,7 @@
         <v>207</v>
       </c>
       <c r="C15" s="70" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D15" s="70"/>
       <c r="E15" s="70" t="s">
@@ -55403,7 +55411,7 @@
         <v>212</v>
       </c>
       <c r="C16" s="75" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D16" s="75"/>
       <c r="E16" s="75" t="s">
@@ -55427,7 +55435,7 @@
         <v>189</v>
       </c>
       <c r="C17" s="70" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D17" s="70"/>
       <c r="E17" s="70" t="s">
@@ -55451,7 +55459,7 @@
         <v>194</v>
       </c>
       <c r="C18" s="75" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D18" s="75"/>
       <c r="E18" s="75" t="s">
@@ -55475,7 +55483,7 @@
         <v>207</v>
       </c>
       <c r="C19" s="70" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D19" s="70"/>
       <c r="E19" s="70" t="s">
@@ -55499,7 +55507,7 @@
         <v>212</v>
       </c>
       <c r="C20" s="75" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D20" s="75"/>
       <c r="E20" s="75" t="s">
@@ -57814,7 +57822,7 @@
   <dimension ref="A1:AE75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L27" sqref="L27"/>
+      <selection activeCell="C5" sqref="C5:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -57860,7 +57868,7 @@
         <v>239</v>
       </c>
       <c r="C5" s="70" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D5" s="70"/>
       <c r="E5" s="70" t="s">
@@ -57898,7 +57906,7 @@
         <v>240</v>
       </c>
       <c r="C6" s="75" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D6" s="75"/>
       <c r="E6" s="75" t="s">
@@ -57940,7 +57948,7 @@
         <v>239</v>
       </c>
       <c r="C7" s="70" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D7" s="70"/>
       <c r="E7" s="70" t="s">
@@ -57983,7 +57991,7 @@
         <v>240</v>
       </c>
       <c r="C8" s="75" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D8" s="75"/>
       <c r="E8" s="75" t="s">
@@ -58007,7 +58015,7 @@
         <v>239</v>
       </c>
       <c r="C9" s="70" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D9" s="70"/>
       <c r="E9" s="70" t="s">
@@ -58031,7 +58039,7 @@
         <v>240</v>
       </c>
       <c r="C10" s="75" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D10" s="75"/>
       <c r="E10" s="75" t="s">
@@ -58067,7 +58075,7 @@
         <v>239</v>
       </c>
       <c r="C11" s="70" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D11" s="70"/>
       <c r="E11" s="70" t="s">
@@ -58110,7 +58118,7 @@
         <v>240</v>
       </c>
       <c r="C12" s="75" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D12" s="75"/>
       <c r="E12" s="75" t="s">
@@ -60646,8 +60654,8 @@
   </sheetPr>
   <dimension ref="B4:R28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L27" sqref="L27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -60695,7 +60703,7 @@
         <v>307</v>
       </c>
       <c r="C5" s="70" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D5" s="70"/>
       <c r="E5" s="70" t="s">
@@ -60742,7 +60750,7 @@
         <v>307</v>
       </c>
       <c r="C6" s="75" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D6" s="75"/>
       <c r="E6" s="75" t="s">
@@ -60789,7 +60797,7 @@
         <v>307</v>
       </c>
       <c r="C7" s="70" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D7" s="70"/>
       <c r="E7" s="70" t="s">
@@ -60836,7 +60844,7 @@
         <v>307</v>
       </c>
       <c r="C8" s="75" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D8" s="75"/>
       <c r="E8" s="75" t="s">
@@ -60883,7 +60891,7 @@
         <v>308</v>
       </c>
       <c r="C9" s="70" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D9" s="70"/>
       <c r="E9" s="70" t="s">
@@ -60930,7 +60938,7 @@
         <v>308</v>
       </c>
       <c r="C10" s="75" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D10" s="75"/>
       <c r="E10" s="75" t="s">
@@ -60977,7 +60985,7 @@
         <v>308</v>
       </c>
       <c r="C11" s="70" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D11" s="70"/>
       <c r="E11" s="70" t="s">
@@ -61004,7 +61012,7 @@
         <v>308</v>
       </c>
       <c r="C12" s="75" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D12" s="75"/>
       <c r="E12" s="75" t="s">
@@ -61031,7 +61039,7 @@
         <v>309</v>
       </c>
       <c r="C13" s="70" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D13" s="70"/>
       <c r="E13" s="70" t="s">
@@ -61058,7 +61066,7 @@
         <v>309</v>
       </c>
       <c r="C14" s="75" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D14" s="75"/>
       <c r="E14" s="75" t="s">
@@ -61085,7 +61093,7 @@
         <v>309</v>
       </c>
       <c r="C15" s="70" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D15" s="70"/>
       <c r="E15" s="70" t="s">
@@ -61112,7 +61120,7 @@
         <v>309</v>
       </c>
       <c r="C16" s="75" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D16" s="75"/>
       <c r="E16" s="75" t="s">
@@ -61139,7 +61147,7 @@
         <v>310</v>
       </c>
       <c r="C17" s="70" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D17" s="70"/>
       <c r="E17" s="70" t="s">
@@ -61166,7 +61174,7 @@
         <v>310</v>
       </c>
       <c r="C18" s="75" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D18" s="75"/>
       <c r="E18" s="75" t="s">
@@ -61193,7 +61201,7 @@
         <v>310</v>
       </c>
       <c r="C19" s="70" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D19" s="70"/>
       <c r="E19" s="70" t="s">
@@ -61220,7 +61228,7 @@
         <v>310</v>
       </c>
       <c r="C20" s="75" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D20" s="75"/>
       <c r="E20" s="75" t="s">
@@ -61247,7 +61255,7 @@
         <v>311</v>
       </c>
       <c r="C21" s="70" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D21" s="70"/>
       <c r="E21" s="70" t="s">
@@ -61274,7 +61282,7 @@
         <v>311</v>
       </c>
       <c r="C22" s="75" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D22" s="75"/>
       <c r="E22" s="75" t="s">
@@ -61301,7 +61309,7 @@
         <v>311</v>
       </c>
       <c r="C23" s="70" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D23" s="70"/>
       <c r="E23" s="70" t="s">
@@ -61328,7 +61336,7 @@
         <v>311</v>
       </c>
       <c r="C24" s="75" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D24" s="75"/>
       <c r="E24" s="75" t="s">
@@ -61355,7 +61363,7 @@
         <v>306</v>
       </c>
       <c r="C25" s="70" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D25" s="70"/>
       <c r="E25" s="70" t="s">
@@ -61382,7 +61390,7 @@
         <v>306</v>
       </c>
       <c r="C26" s="75" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D26" s="75"/>
       <c r="E26" s="75" t="s">
@@ -61409,7 +61417,7 @@
         <v>306</v>
       </c>
       <c r="C27" s="70" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D27" s="70"/>
       <c r="E27" s="70" t="s">
@@ -61436,7 +61444,7 @@
         <v>306</v>
       </c>
       <c r="C28" s="75" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="D28" s="75"/>
       <c r="E28" s="75" t="s">

</xml_diff>